<commit_message>
Worked on TC05 - Self Services, 04 - Tickets Test Cases (TC_050 - TC_055), and add Test Data to TC_053
</commit_message>
<xml_diff>
--- a/Empxtrack_Nafis/Data Files/Test Data.xlsx
+++ b/Empxtrack_Nafis/Data Files/Test Data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7650" activeTab="1"/>
+    <workbookView windowWidth="20490" windowHeight="7650" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TC04-01-013 Add New Event" sheetId="1" r:id="rId1"/>
     <sheet name="TC04-01-015 Add New Task" sheetId="2" r:id="rId2"/>
+    <sheet name="TC05-04-053 AddMyTicket" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>subject</t>
   </si>
@@ -180,6 +181,42 @@
   </si>
   <si>
     <t>emp 03</t>
+  </si>
+  <si>
+    <t>ticketType</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>expectedDate</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>05/02/2024</t>
+  </si>
+  <si>
+    <t>Ticket 1saa</t>
+  </si>
+  <si>
+    <t>issa ticket</t>
+  </si>
+  <si>
+    <t>C:\Users\Hasnul\Katalon Studio\Katalon-Studio-Training-Assessment\Empxtrack_Nafis\File Upload Test Data\Katalon Studio Training Day 2.pdf</t>
+  </si>
+  <si>
+    <t>Ticket 2aa</t>
+  </si>
+  <si>
+    <t>issa ticketttttt</t>
   </si>
 </sst>
 </file>
@@ -193,14 +230,7 @@
     <numFmt numFmtId="179" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="0.0"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,148 +686,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1420,7 +1450,7 @@
   <sheetPr/>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -1493,4 +1523,81 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>